<commit_message>
implemented ClearCart... implemented GerMaxOrderValue... implemented 'chopping of queues'...
</commit_message>
<xml_diff>
--- a/Project_3/Data/Orders2.xlsx
+++ b/Project_3/Data/Orders2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69D1FAEB-217C-4D18-92D6-328896C34014}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB60983C-9C52-4BDD-8F07-A47E93AB2F03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -89,9 +89,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Beverage</t>
-  </si>
-  <si>
     <t>Aniseed Syrup</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Beverages</t>
   </si>
 </sst>
 </file>
@@ -468,16 +468,16 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -502,11 +502,11 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -514,21 +514,21 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -536,10 +536,10 @@
         <v>12.7</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -547,21 +547,21 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1">
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -569,10 +569,10 @@
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -580,21 +580,21 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -602,152 +602,152 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1">
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1">
         <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15">
         <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21">
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>25.5</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -764,17 +764,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -794,7 +794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>